<commit_message>
Change Files and Models to have correct names
</commit_message>
<xml_diff>
--- a/data/gameStats.xlsx
+++ b/data/gameStats.xlsx
@@ -43,6 +43,252 @@
     <t>MatchKD</t>
   </si>
   <si>
+    <t>London Royal Ravens</t>
+  </si>
+  <si>
+    <t>Obaid Asim</t>
+  </si>
+  <si>
+    <t>Asim</t>
+  </si>
+  <si>
+    <t>Matthew Marshall</t>
+  </si>
+  <si>
+    <t>Skrapz</t>
+  </si>
+  <si>
+    <t>Byron Plumridge</t>
+  </si>
+  <si>
+    <t>Nastie</t>
+  </si>
+  <si>
+    <t>Ulisses  Rios</t>
+  </si>
+  <si>
+    <t>Uli</t>
+  </si>
+  <si>
+    <t>Los Angeles Thieves</t>
+  </si>
+  <si>
+    <t>Kenneth Williams</t>
+  </si>
+  <si>
+    <t>Kenny</t>
+  </si>
+  <si>
+    <t>Sam Larew</t>
+  </si>
+  <si>
+    <t>Octane</t>
+  </si>
+  <si>
+    <t>Dylan Hannon</t>
+  </si>
+  <si>
+    <t>Envoy</t>
+  </si>
+  <si>
+    <t>Zachary Jordan</t>
+  </si>
+  <si>
+    <t>Drazah</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Vegas Legion</t>
+  </si>
+  <si>
+    <t>James Eubanks</t>
+  </si>
+  <si>
+    <t>Clayster</t>
+  </si>
+  <si>
+    <t>Donovan Laroda</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>Thomas  Haly</t>
+  </si>
+  <si>
+    <t>TJHaLy</t>
+  </si>
+  <si>
+    <t>Eli Bentz</t>
+  </si>
+  <si>
+    <t>Standy</t>
+  </si>
+  <si>
+    <t>Boston Breach</t>
+  </si>
+  <si>
+    <t>Reece Drost</t>
+  </si>
+  <si>
+    <t>Vivid</t>
+  </si>
+  <si>
+    <t>Joseph Conley</t>
+  </si>
+  <si>
+    <t>Owakening</t>
+  </si>
+  <si>
+    <t>Dylan Koch</t>
+  </si>
+  <si>
+    <t>Nero</t>
+  </si>
+  <si>
+    <t>Ben McMellon</t>
+  </si>
+  <si>
+    <t>Beans</t>
+  </si>
+  <si>
+    <t>Florida Mutineers</t>
+  </si>
+  <si>
+    <t>Carson Newberry</t>
+  </si>
+  <si>
+    <t>Brack</t>
+  </si>
+  <si>
+    <t>Colt McLendon</t>
+  </si>
+  <si>
+    <t>Havok</t>
+  </si>
+  <si>
+    <t>Tyler Johnson</t>
+  </si>
+  <si>
+    <t>FeLo</t>
+  </si>
+  <si>
+    <t>Kenyen Sutton</t>
+  </si>
+  <si>
+    <t>Capsidal</t>
+  </si>
+  <si>
+    <t>Minnesota Røkkr</t>
+  </si>
+  <si>
+    <t>Benjamin Bance</t>
+  </si>
+  <si>
+    <t>Bance</t>
+  </si>
+  <si>
+    <t>Cameron McKilligan</t>
+  </si>
+  <si>
+    <t>Cammy</t>
+  </si>
+  <si>
+    <t>Marcus Reid</t>
+  </si>
+  <si>
+    <t>Afro</t>
+  </si>
+  <si>
+    <t>Kevin  Bonanno</t>
+  </si>
+  <si>
+    <t>Fame</t>
+  </si>
+  <si>
+    <t>Toronto Ultra</t>
+  </si>
+  <si>
+    <t>Tobias Juul Jønsson</t>
+  </si>
+  <si>
+    <t>CleanX</t>
+  </si>
+  <si>
+    <t>Jamie Craven</t>
+  </si>
+  <si>
+    <t>Insight</t>
+  </si>
+  <si>
+    <t>Charlie Hicks</t>
+  </si>
+  <si>
+    <t>Hicksy</t>
+  </si>
+  <si>
+    <t>Thomas Ernst</t>
+  </si>
+  <si>
+    <t>Scrap</t>
+  </si>
+  <si>
+    <t>Los Angeles Guerrillas</t>
+  </si>
+  <si>
+    <t>Adam Garcia</t>
+  </si>
+  <si>
+    <t>Assault</t>
+  </si>
+  <si>
+    <t>Alec Sanderson</t>
+  </si>
+  <si>
+    <t>Arcitys</t>
+  </si>
+  <si>
+    <t>Kaden Stockdale</t>
+  </si>
+  <si>
+    <t>Exceed</t>
+  </si>
+  <si>
+    <t>Joseph Romero</t>
+  </si>
+  <si>
+    <t>JoeDeceives</t>
+  </si>
+  <si>
+    <t>Seattle Surge</t>
+  </si>
+  <si>
+    <t>Lamar Abedi</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Makenzie Kelley</t>
+  </si>
+  <si>
+    <t>Mack</t>
+  </si>
+  <si>
+    <t>Daunte Gray</t>
+  </si>
+  <si>
+    <t>Sib</t>
+  </si>
+  <si>
+    <t>Amer Zulbeari</t>
+  </si>
+  <si>
+    <t>Pred</t>
+  </si>
+  <si>
     <t>New York Subliners</t>
   </si>
   <si>
@@ -95,252 +341,6 @@
   </si>
   <si>
     <t>SlasheR</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Vegas Legion</t>
-  </si>
-  <si>
-    <t>James Eubanks</t>
-  </si>
-  <si>
-    <t>Clayster</t>
-  </si>
-  <si>
-    <t>Donovan Laroda</t>
-  </si>
-  <si>
-    <t>Temp</t>
-  </si>
-  <si>
-    <t>Thomas  Haly</t>
-  </si>
-  <si>
-    <t>TJHaLy</t>
-  </si>
-  <si>
-    <t>Eli Bentz</t>
-  </si>
-  <si>
-    <t>Standy</t>
-  </si>
-  <si>
-    <t>Boston Breach</t>
-  </si>
-  <si>
-    <t>Reece Drost</t>
-  </si>
-  <si>
-    <t>Vivid</t>
-  </si>
-  <si>
-    <t>Joseph Conley</t>
-  </si>
-  <si>
-    <t>Owakening</t>
-  </si>
-  <si>
-    <t>Dylan Koch</t>
-  </si>
-  <si>
-    <t>Nero</t>
-  </si>
-  <si>
-    <t>Ben McMellon</t>
-  </si>
-  <si>
-    <t>Beans</t>
-  </si>
-  <si>
-    <t>Seattle Surge</t>
-  </si>
-  <si>
-    <t>Lamar Abedi</t>
-  </si>
-  <si>
-    <t>Accuracy</t>
-  </si>
-  <si>
-    <t>Makenzie Kelley</t>
-  </si>
-  <si>
-    <t>Mack</t>
-  </si>
-  <si>
-    <t>Daunte Gray</t>
-  </si>
-  <si>
-    <t>Sib</t>
-  </si>
-  <si>
-    <t>Amer Zulbeari</t>
-  </si>
-  <si>
-    <t>Pred</t>
-  </si>
-  <si>
-    <t>Los Angeles Thieves</t>
-  </si>
-  <si>
-    <t>Kenneth Williams</t>
-  </si>
-  <si>
-    <t>Kenny</t>
-  </si>
-  <si>
-    <t>Sam Larew</t>
-  </si>
-  <si>
-    <t>Octane</t>
-  </si>
-  <si>
-    <t>Dylan Hannon</t>
-  </si>
-  <si>
-    <t>Envoy</t>
-  </si>
-  <si>
-    <t>Zachary Jordan</t>
-  </si>
-  <si>
-    <t>Drazah</t>
-  </si>
-  <si>
-    <t>Minnesota Røkkr</t>
-  </si>
-  <si>
-    <t>Benjamin Bance</t>
-  </si>
-  <si>
-    <t>Bance</t>
-  </si>
-  <si>
-    <t>Cameron McKilligan</t>
-  </si>
-  <si>
-    <t>Cammy</t>
-  </si>
-  <si>
-    <t>Marcus Reid</t>
-  </si>
-  <si>
-    <t>Afro</t>
-  </si>
-  <si>
-    <t>Kevin  Bonanno</t>
-  </si>
-  <si>
-    <t>Fame</t>
-  </si>
-  <si>
-    <t>Los Angeles Guerrillas</t>
-  </si>
-  <si>
-    <t>Adam Garcia</t>
-  </si>
-  <si>
-    <t>Assault</t>
-  </si>
-  <si>
-    <t>Alec Sanderson</t>
-  </si>
-  <si>
-    <t>Arcitys</t>
-  </si>
-  <si>
-    <t>Kaden Stockdale</t>
-  </si>
-  <si>
-    <t>Exceed</t>
-  </si>
-  <si>
-    <t>Joseph Romero</t>
-  </si>
-  <si>
-    <t>JoeDeceives</t>
-  </si>
-  <si>
-    <t>Toronto Ultra</t>
-  </si>
-  <si>
-    <t>Tobias Juul Jønsson</t>
-  </si>
-  <si>
-    <t>CleanX</t>
-  </si>
-  <si>
-    <t>Jamie Craven</t>
-  </si>
-  <si>
-    <t>Insight</t>
-  </si>
-  <si>
-    <t>Charlie Hicks</t>
-  </si>
-  <si>
-    <t>Hicksy</t>
-  </si>
-  <si>
-    <t>Thomas Ernst</t>
-  </si>
-  <si>
-    <t>Scrap</t>
-  </si>
-  <si>
-    <t>London Royal Ravens</t>
-  </si>
-  <si>
-    <t>Obaid Asim</t>
-  </si>
-  <si>
-    <t>Asim</t>
-  </si>
-  <si>
-    <t>Matthew Marshall</t>
-  </si>
-  <si>
-    <t>Skrapz</t>
-  </si>
-  <si>
-    <t>Byron Plumridge</t>
-  </si>
-  <si>
-    <t>Nastie</t>
-  </si>
-  <si>
-    <t>Ulisses  Rios</t>
-  </si>
-  <si>
-    <t>Uli</t>
-  </si>
-  <si>
-    <t>Florida Mutineers</t>
-  </si>
-  <si>
-    <t>Carson Newberry</t>
-  </si>
-  <si>
-    <t>Brack</t>
-  </si>
-  <si>
-    <t>Colt McLendon</t>
-  </si>
-  <si>
-    <t>Havok</t>
-  </si>
-  <si>
-    <t>Tyler Johnson</t>
-  </si>
-  <si>
-    <t>FeLo</t>
-  </si>
-  <si>
-    <t>Kenyen Sutton</t>
-  </si>
-  <si>
-    <t>Capsidal</t>
   </si>
 </sst>
 </file>
@@ -761,7 +761,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>8769</v>
+        <v>8761</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -773,27 +773,27 @@
         <v>12</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="F2">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="G2">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="H2">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="I2">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="J2">
-        <v>1.28</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>8769</v>
+        <v>8761</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -805,27 +805,27 @@
         <v>14</v>
       </c>
       <c r="E3">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="F3">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="G3">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <v>19</v>
+      </c>
+      <c r="I3">
         <v>24</v>
       </c>
-      <c r="H3">
-        <v>66</v>
-      </c>
-      <c r="I3">
-        <v>226</v>
-      </c>
       <c r="J3">
-        <v>1.23</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>8769</v>
+        <v>8761</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -837,27 +837,27 @@
         <v>16</v>
       </c>
       <c r="E4">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="F4">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="G4">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="H4">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="I4">
-        <v>104</v>
+        <v>19</v>
       </c>
       <c r="J4">
-        <v>0.86</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>8769</v>
+        <v>8761</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -869,27 +869,27 @@
         <v>18</v>
       </c>
       <c r="E5">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="F5">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="G5">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H5">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="I5">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="J5">
-        <v>0.88</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>8769</v>
+        <v>8761</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -901,27 +901,27 @@
         <v>21</v>
       </c>
       <c r="E6">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="F6">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="G6">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H6">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="I6">
-        <v>224</v>
+        <v>41</v>
       </c>
       <c r="J6">
-        <v>1.15</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>8769</v>
+        <v>8761</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -933,27 +933,27 @@
         <v>23</v>
       </c>
       <c r="E7">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="F7">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="G7">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H7">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="I7">
-        <v>45</v>
+        <v>140</v>
       </c>
       <c r="J7">
-        <v>0.91</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8769</v>
+        <v>8761</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -965,27 +965,27 @@
         <v>25</v>
       </c>
       <c r="E8">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="F8">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="G8">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="H8">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="I8">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J8">
-        <v>1.06</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8769</v>
+        <v>8761</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
@@ -997,22 +997,22 @@
         <v>27</v>
       </c>
       <c r="E9">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="F9">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="G9">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="H9">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="I9">
-        <v>173</v>
+        <v>47</v>
       </c>
       <c r="J9">
-        <v>0.71</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1337,7 +1337,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>8766</v>
+        <v>8763</v>
       </c>
       <c r="B20" t="s">
         <v>47</v>
@@ -1349,27 +1349,27 @@
         <v>49</v>
       </c>
       <c r="E20">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F20">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G20">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H20">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I20">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="J20">
-        <v>1.11</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>8766</v>
+        <v>8763</v>
       </c>
       <c r="B21" t="s">
         <v>47</v>
@@ -1381,27 +1381,27 @@
         <v>51</v>
       </c>
       <c r="E21">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="F21">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="G21">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="H21">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="I21">
         <v>58</v>
       </c>
       <c r="J21">
-        <v>0.72</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>8766</v>
+        <v>8763</v>
       </c>
       <c r="B22" t="s">
         <v>47</v>
@@ -1413,27 +1413,27 @@
         <v>53</v>
       </c>
       <c r="E22">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="F22">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G22">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H22">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I22">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="J22">
-        <v>0.81</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>8766</v>
+        <v>8763</v>
       </c>
       <c r="B23" t="s">
         <v>47</v>
@@ -1445,27 +1445,27 @@
         <v>55</v>
       </c>
       <c r="E23">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="F23">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="G23">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H23">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="I23">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="J23">
-        <v>1.07</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>8766</v>
+        <v>8763</v>
       </c>
       <c r="B24" t="s">
         <v>56</v>
@@ -1477,27 +1477,27 @@
         <v>58</v>
       </c>
       <c r="E24">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="F24">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G24">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H24">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="I24">
-        <v>109</v>
+        <v>27</v>
       </c>
       <c r="J24">
-        <v>1.1</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>8766</v>
+        <v>8763</v>
       </c>
       <c r="B25" t="s">
         <v>56</v>
@@ -1509,27 +1509,27 @@
         <v>60</v>
       </c>
       <c r="E25">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F25">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G25">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H25">
         <v>42</v>
       </c>
       <c r="I25">
-        <v>128</v>
+        <v>60</v>
       </c>
       <c r="J25">
-        <v>1.14</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>8766</v>
+        <v>8763</v>
       </c>
       <c r="B26" t="s">
         <v>56</v>
@@ -1541,27 +1541,27 @@
         <v>62</v>
       </c>
       <c r="E26">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="F26">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="G26">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H26">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="I26">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="J26">
-        <v>1.46</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>8766</v>
+        <v>8763</v>
       </c>
       <c r="B27" t="s">
         <v>56</v>
@@ -1573,22 +1573,22 @@
         <v>64</v>
       </c>
       <c r="E27">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="F27">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="G27">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="H27">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="I27">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="J27">
-        <v>0.95</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1625,7 +1625,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>8765</v>
+        <v>8764</v>
       </c>
       <c r="B29" t="s">
         <v>65</v>
@@ -1637,27 +1637,27 @@
         <v>67</v>
       </c>
       <c r="E29">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="F29">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="G29">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="H29">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="I29">
-        <v>145</v>
+        <v>87</v>
       </c>
       <c r="J29">
-        <v>0.75</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>8765</v>
+        <v>8764</v>
       </c>
       <c r="B30" t="s">
         <v>65</v>
@@ -1669,27 +1669,27 @@
         <v>69</v>
       </c>
       <c r="E30">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="F30">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G30">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="H30">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="I30">
-        <v>97</v>
+        <v>183</v>
       </c>
       <c r="J30">
-        <v>0.77</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>8765</v>
+        <v>8764</v>
       </c>
       <c r="B31" t="s">
         <v>65</v>
@@ -1701,27 +1701,27 @@
         <v>71</v>
       </c>
       <c r="E31">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F31">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="G31">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="H31">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="I31">
-        <v>95</v>
+        <v>191</v>
       </c>
       <c r="J31">
-        <v>1.18</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>8765</v>
+        <v>8764</v>
       </c>
       <c r="B32" t="s">
         <v>65</v>
@@ -1733,150 +1733,150 @@
         <v>73</v>
       </c>
       <c r="E32">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="F32">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="G32">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="H32">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="I32">
-        <v>138</v>
+        <v>86</v>
       </c>
       <c r="J32">
-        <v>0.99</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>8765</v>
+        <v>8764</v>
       </c>
       <c r="B33" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="E33">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="F33">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="G33">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H33">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="I33">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="J33">
-        <v>0.92</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>8765</v>
+        <v>8764</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="E34">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F34">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="G34">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H34">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I34">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J34">
-        <v>1.12</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>8765</v>
+        <v>8764</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="E35">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="F35">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="G35">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H35">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="I35">
-        <v>90</v>
+        <v>129</v>
       </c>
       <c r="J35">
-        <v>0.91</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>8765</v>
+        <v>8764</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="D36" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="E36">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="F36">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="G36">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H36">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="I36">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="J36">
-        <v>1.46</v>
+        <v>1.11</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -1913,258 +1913,258 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>8764</v>
+        <v>8765</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="D38" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="E38">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="F38">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="G38">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="H38">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="I38">
-        <v>87</v>
+        <v>145</v>
       </c>
       <c r="J38">
-        <v>0.94</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>8764</v>
+        <v>8765</v>
       </c>
       <c r="B39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39">
+        <v>64</v>
+      </c>
+      <c r="F39">
         <v>83</v>
       </c>
-      <c r="C39" t="s">
-        <v>86</v>
-      </c>
-      <c r="D39" t="s">
-        <v>87</v>
-      </c>
-      <c r="E39">
-        <v>73</v>
-      </c>
-      <c r="F39">
-        <v>82</v>
-      </c>
       <c r="G39">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="H39">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="I39">
-        <v>183</v>
+        <v>97</v>
       </c>
       <c r="J39">
-        <v>0.89</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>8764</v>
+        <v>8765</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C40" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="D40" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="E40">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F40">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="G40">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="H40">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="I40">
-        <v>191</v>
+        <v>95</v>
       </c>
       <c r="J40">
-        <v>0.86</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>8764</v>
+        <v>8765</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="D41" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="E41">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="F41">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="G41">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="H41">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="I41">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="J41">
-        <v>1.05</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>8764</v>
+        <v>8765</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="C42" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="D42" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="E42">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="F42">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="G42">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H42">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="I42">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="J42">
-        <v>1.14</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>8764</v>
+        <v>8765</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="C43" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="E43">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F43">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G43">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H43">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="I43">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="J43">
-        <v>1.06</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>8764</v>
+        <v>8765</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="C44" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="D44" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="E44">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="F44">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="G44">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H44">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="I44">
-        <v>129</v>
+        <v>90</v>
       </c>
       <c r="J44">
-        <v>0.99</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>8764</v>
+        <v>8765</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="D45" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="E45">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="F45">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="G45">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H45">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="I45">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="J45">
-        <v>1.11</v>
+        <v>1.46</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2201,258 +2201,258 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>8761</v>
+        <v>8766</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C47" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D47" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E47">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="F47">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="G47">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="H47">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="I47">
-        <v>33</v>
+        <v>156</v>
       </c>
       <c r="J47">
-        <v>0.73</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>8761</v>
+        <v>8766</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C48" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D48" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E48">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="F48">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="G48">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="H48">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="I48">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="J48">
-        <v>0.66</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>8761</v>
+        <v>8766</v>
       </c>
       <c r="B49" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C49" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D49" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E49">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="F49">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="G49">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="H49">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="I49">
-        <v>19</v>
+        <v>134</v>
       </c>
       <c r="J49">
-        <v>0.71</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>8761</v>
+        <v>8766</v>
       </c>
       <c r="B50" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C50" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D50" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E50">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="F50">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="G50">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="H50">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="I50">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="J50">
-        <v>0.78</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>8761</v>
+        <v>8766</v>
       </c>
       <c r="B51" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C51" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="D51" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="E51">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="F51">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="G51">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="H51">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="I51">
-        <v>41</v>
+        <v>109</v>
       </c>
       <c r="J51">
-        <v>1.59</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>8761</v>
+        <v>8766</v>
       </c>
       <c r="B52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52">
+        <v>76</v>
+      </c>
+      <c r="F52">
+        <v>72</v>
+      </c>
+      <c r="G52">
+        <v>25</v>
+      </c>
+      <c r="H52">
         <v>56</v>
       </c>
-      <c r="C52" t="s">
-        <v>59</v>
-      </c>
-      <c r="D52" t="s">
-        <v>60</v>
-      </c>
-      <c r="E52">
-        <v>31</v>
-      </c>
-      <c r="F52">
-        <v>29</v>
-      </c>
-      <c r="G52">
-        <v>11</v>
-      </c>
-      <c r="H52">
-        <v>22</v>
-      </c>
       <c r="I52">
-        <v>140</v>
+        <v>218</v>
       </c>
       <c r="J52">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>8761</v>
+        <v>8766</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="D53" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="E53">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="F53">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="G53">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="H53">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="I53">
-        <v>62</v>
+        <v>130</v>
       </c>
       <c r="J53">
-        <v>1.26</v>
+        <v>1.46</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>8761</v>
+        <v>8766</v>
       </c>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C54" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="D54" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="E54">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="F54">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="G54">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="H54">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="I54">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="J54">
-        <v>1.69</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -2489,258 +2489,258 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>8763</v>
+        <v>8769</v>
       </c>
       <c r="B56" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C56" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D56" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E56">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="F56">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="G56">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="H56">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="I56">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="J56">
-        <v>1.26</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>8763</v>
+        <v>8769</v>
       </c>
       <c r="B57" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C57" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D57" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E57">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="F57">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="G57">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="H57">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="I57">
-        <v>58</v>
+        <v>226</v>
       </c>
       <c r="J57">
-        <v>0.82</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>8763</v>
+        <v>8769</v>
       </c>
       <c r="B58" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C58" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D58" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E58">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="F58">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="G58">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="H58">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="I58">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="J58">
-        <v>0.98</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>8763</v>
+        <v>8769</v>
       </c>
       <c r="B59" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C59" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D59" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E59">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="F59">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="G59">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H59">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="I59">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="J59">
-        <v>0.51</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>8763</v>
+        <v>8769</v>
       </c>
       <c r="B60" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="C60" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="D60" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="E60">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="F60">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="G60">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H60">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="I60">
-        <v>27</v>
+        <v>224</v>
       </c>
       <c r="J60">
-        <v>0.82</v>
+        <v>1.15</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>8763</v>
+        <v>8769</v>
       </c>
       <c r="B61" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="C61" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="D61" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="E61">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="F61">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="G61">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="H61">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="I61">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="J61">
-        <v>1.16</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>8763</v>
+        <v>8769</v>
       </c>
       <c r="B62" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="C62" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="D62" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="E62">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="F62">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="G62">
         <v>21</v>
       </c>
       <c r="H62">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="I62">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="J62">
-        <v>1.33</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>8763</v>
+        <v>8769</v>
       </c>
       <c r="B63" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="C63" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="D63" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="E63">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F63">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="G63">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="H63">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I63">
-        <v>99</v>
+        <v>173</v>
       </c>
       <c r="J63">
-        <v>1.5</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>